<commit_message>
Scripts to find non-projective sentences.
</commit_message>
<xml_diff>
--- a/Projectivity/linear_order_analysis.xlsx
+++ b/Projectivity/linear_order_analysis.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="25">
   <si>
     <t>doctus</t>
   </si>
@@ -1206,10 +1206,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I166" sqref="I166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H81">
         <f>COUNTIF(H3:H78,"np")</f>
         <v>12</v>
@@ -2702,8 +2703,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="2:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>16</v>
       </c>
@@ -2717,74 +2718,1442 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>16</v>
-      </c>
-      <c r="C87" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>15</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>3</v>
+      </c>
+      <c r="G87">
+        <f>SUM(B87:E87)</f>
+        <v>5</v>
+      </c>
+      <c r="H87" t="s">
+        <v>4</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <f>SUM(B88:E88)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89" t="s">
         <v>22</v>
       </c>
-      <c r="D87" t="s">
-        <v>18</v>
-      </c>
-      <c r="E87" t="s">
+      <c r="D89" t="s">
+        <v>18</v>
+      </c>
+      <c r="E89" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>16</v>
-      </c>
-      <c r="C88" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="G90">
+        <f t="shared" ref="G90:G123" si="4">SUM(B90:E90)</f>
+        <v>5</v>
+      </c>
+      <c r="H90" t="s">
+        <v>5</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" t="s">
         <v>24</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D92" t="s">
         <v>22</v>
       </c>
-      <c r="E88" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>16</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="E92" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>15</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H93" t="s">
+        <v>4</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" t="s">
         <v>24</v>
       </c>
-      <c r="D89" t="s">
-        <v>18</v>
-      </c>
-      <c r="E89" t="s">
+      <c r="D95" t="s">
+        <v>18</v>
+      </c>
+      <c r="E95" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>16</v>
-      </c>
-      <c r="C90" t="s">
-        <v>18</v>
-      </c>
-      <c r="D90" t="s">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+      <c r="E96">
+        <v>3</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="H96" t="s">
+        <v>5</v>
+      </c>
+      <c r="I96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>20</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" t="s">
         <v>22</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E98" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>16</v>
-      </c>
-      <c r="C91" t="s">
-        <v>18</v>
-      </c>
-      <c r="D91" t="s">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>15</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H99" t="s">
+        <v>4</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101" t="s">
         <v>23</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E101" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>15</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>3</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H102" t="s">
+        <v>4</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106" t="s">
+        <v>16</v>
+      </c>
+      <c r="D106" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>15</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+      <c r="E107">
+        <v>2</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H107" t="s">
+        <v>5</v>
+      </c>
+      <c r="I107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>22</v>
+      </c>
+      <c r="C109" t="s">
+        <v>16</v>
+      </c>
+      <c r="D109" t="s">
+        <v>18</v>
+      </c>
+      <c r="E109" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>15</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>3</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H110" t="s">
+        <v>5</v>
+      </c>
+      <c r="I110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>22</v>
+      </c>
+      <c r="C112" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" t="s">
+        <v>16</v>
+      </c>
+      <c r="E112" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>15</v>
+      </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H113" t="s">
+        <v>4</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>20</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>22</v>
+      </c>
+      <c r="C115" t="s">
+        <v>24</v>
+      </c>
+      <c r="D115" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>15</v>
+      </c>
+      <c r="B116">
+        <v>3</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H116" t="s">
+        <v>4</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>20</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>22</v>
+      </c>
+      <c r="C118" t="s">
+        <v>18</v>
+      </c>
+      <c r="D118" t="s">
+        <v>16</v>
+      </c>
+      <c r="E118" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>15</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>3</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H119" t="s">
+        <v>5</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>20</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>22</v>
+      </c>
+      <c r="C121" t="s">
+        <v>18</v>
+      </c>
+      <c r="D121" t="s">
+        <v>24</v>
+      </c>
+      <c r="E121" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>15</v>
+      </c>
+      <c r="B122">
+        <v>3</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <v>2</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="H122" t="s">
+        <v>5</v>
+      </c>
+      <c r="I122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>20</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>24</v>
+      </c>
+      <c r="C127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127" t="s">
+        <v>22</v>
+      </c>
+      <c r="E127" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>15</v>
+      </c>
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128">
+        <v>2</v>
+      </c>
+      <c r="G128">
+        <f>SUM(B128:E128)</f>
+        <v>5</v>
+      </c>
+      <c r="H128" t="s">
+        <v>5</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>20</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="G129">
+        <f t="shared" ref="G129:G144" si="5">SUM(B129:E129)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>24</v>
+      </c>
+      <c r="C130" t="s">
+        <v>16</v>
+      </c>
+      <c r="D130" t="s">
+        <v>18</v>
+      </c>
+      <c r="E130" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>15</v>
+      </c>
+      <c r="B131">
+        <v>3</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>2</v>
+      </c>
+      <c r="G131">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="H131" t="s">
+        <v>5</v>
+      </c>
+      <c r="I131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>20</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="G132">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>24</v>
+      </c>
+      <c r="C133" t="s">
+        <v>22</v>
+      </c>
+      <c r="D133" t="s">
+        <v>16</v>
+      </c>
+      <c r="E133" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>15</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="G134">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="H134" t="s">
+        <v>4</v>
+      </c>
+      <c r="I134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>20</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="G135">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>24</v>
+      </c>
+      <c r="C136" t="s">
+        <v>22</v>
+      </c>
+      <c r="D136" t="s">
+        <v>18</v>
+      </c>
+      <c r="E136" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>15</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>2</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="G137">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="H137" t="s">
+        <v>4</v>
+      </c>
+      <c r="I137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>20</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>24</v>
+      </c>
+      <c r="C139" t="s">
+        <v>18</v>
+      </c>
+      <c r="D139" t="s">
+        <v>16</v>
+      </c>
+      <c r="E139" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>15</v>
+      </c>
+      <c r="B140">
+        <v>3</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="H140" t="s">
+        <v>5</v>
+      </c>
+      <c r="I140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>20</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>24</v>
+      </c>
+      <c r="C142" t="s">
+        <v>18</v>
+      </c>
+      <c r="D142" t="s">
+        <v>22</v>
+      </c>
+      <c r="E142" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>15</v>
+      </c>
+      <c r="B143">
+        <v>2</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="H143" t="s">
+        <v>5</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>20</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>18</v>
+      </c>
+      <c r="C148" t="s">
+        <v>16</v>
+      </c>
+      <c r="D148" t="s">
+        <v>22</v>
+      </c>
+      <c r="E148" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="G149">
+        <f>SUM(B149:E149)</f>
+        <v>3</v>
+      </c>
+      <c r="H149" t="s">
+        <v>4</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="G150">
+        <f t="shared" ref="G150:G165" si="6">SUM(B150:E150)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>18</v>
+      </c>
+      <c r="C151" t="s">
+        <v>16</v>
+      </c>
+      <c r="D151" t="s">
+        <v>24</v>
+      </c>
+      <c r="E151" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="152" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>2</v>
+      </c>
+      <c r="G152">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="H152" t="s">
+        <v>4</v>
+      </c>
+      <c r="I152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>18</v>
+      </c>
+      <c r="C154" t="s">
+        <v>22</v>
+      </c>
+      <c r="D154" t="s">
+        <v>16</v>
+      </c>
+      <c r="E154" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>2</v>
+      </c>
+      <c r="C155">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>2</v>
+      </c>
+      <c r="G155">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="H155" t="s">
+        <v>5</v>
+      </c>
+      <c r="I155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="G156">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>18</v>
+      </c>
+      <c r="C157" t="s">
+        <v>22</v>
+      </c>
+      <c r="D157" t="s">
+        <v>24</v>
+      </c>
+      <c r="E157" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>3</v>
+      </c>
+      <c r="C158">
+        <v>2</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="G158">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="H158" t="s">
+        <v>4</v>
+      </c>
+      <c r="I158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>18</v>
+      </c>
+      <c r="C160" t="s">
+        <v>24</v>
+      </c>
+      <c r="D160" t="s">
+        <v>16</v>
+      </c>
+      <c r="E160" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="161" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>2</v>
+      </c>
+      <c r="C161">
+        <v>2</v>
+      </c>
+      <c r="D161">
+        <v>0</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="H161" t="s">
+        <v>5</v>
+      </c>
+      <c r="I161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="G162">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>18</v>
+      </c>
+      <c r="C163" t="s">
+        <v>24</v>
+      </c>
+      <c r="D163" t="s">
+        <v>22</v>
+      </c>
+      <c r="E163" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="164" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>3</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>0</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="H164" t="s">
+        <v>4</v>
+      </c>
+      <c r="I164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+      <c r="G165">
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>